<commit_message>
json 변환 dll 추가
</commit_message>
<xml_diff>
--- a/ExcelParsingConverter/bin/Debug/GameTableDoc.xlsx
+++ b/ExcelParsingConverter/bin/Debug/GameTableDoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ninja\ExcelParsing\ExcelParsingConverter\ExcelParsingConverter\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\learnUnity\converts\ExcelParsingConverter\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28DB7635-1148-4101-A8A9-287D7F5BCA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D51344-F474-42D3-A2DD-054147D94F9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-9000" windowWidth="16440" windowHeight="28320" firstSheet="1" xr2:uid="{81A7C282-206D-4EA9-B4CD-D05BD95E55F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{81A7C282-206D-4EA9-B4CD-D05BD95E55F5}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterTable" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -131,7 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,7 +361,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -670,17 +659,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7DB743-F875-4C4B-B987-827B825DF9E9}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1048576"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="15.625" customWidth="1"/>
     <col min="11" max="11" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -715,7 +704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1001</v>
       </c>
@@ -750,7 +739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1002</v>
       </c>
@@ -785,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1003</v>
       </c>
@@ -820,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1004</v>
       </c>
@@ -855,7 +844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.25" thickBot="1">
+    <row r="6" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>1005</v>
       </c>
@@ -901,13 +890,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0084DE02-CF23-4285-82FC-B3AA6CD44AFF}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -930,7 +919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -953,7 +942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -976,7 +965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -999,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1022,7 +1011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1045,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.25" thickBot="1">
+    <row r="7" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>6</v>
       </c>

</xml_diff>